<commit_message>
Fixed tax-aware optimization tax netting allowing positive tax liability (credit)
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\christoph\projects\tax-aware-portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D07832C-E101-40A5-AC67-47FE53312209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C315AB-D53E-4530-AE17-F5FC4B9D5274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{479A00DE-E2FA-4AAC-9746-77087B1E4B23}"/>
   </bookViews>
@@ -174,9 +174,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -308,38 +309,33 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -656,21 +652,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A066EE-72B8-43A0-A297-501044A2E4E1}">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="26"/>
     <col min="20" max="20" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -678,46 +674,46 @@
         <v>45756</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S2" t="s">
         <v>29</v>
       </c>
       <c r="T2" t="s">
         <v>32</v>
       </c>
-      <c r="V2" t="s">
+      <c r="U2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="15" t="s">
         <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
       <c r="K3" t="s">
@@ -740,317 +736,311 @@
       </c>
       <c r="S3">
         <f>SUMIF(N4:N7,"=short term",O4:O7)</f>
-        <v>28.333333140137206</v>
-      </c>
-      <c r="T3" s="27">
+        <v>19.298245125612038</v>
+      </c>
+      <c r="T3" s="22">
         <f>IF(S3*S4&lt;0,IF(S3&gt;-S4,S3+S4,0),S3)</f>
-        <v>0</v>
-      </c>
-      <c r="V3">
+        <v>19.298245125612038</v>
+      </c>
+      <c r="U3">
         <f>T3*0.35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+        <v>6.7543857939642127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>10</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>190</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="14">
         <f>$B$1-400</f>
         <v>45356</v>
       </c>
-      <c r="F4" s="17">
-        <v>180</v>
-      </c>
-      <c r="G4" s="13">
+      <c r="F4" s="12">
+        <v>200</v>
+      </c>
+      <c r="G4" s="11">
         <f>C4*F4/SUMPRODUCT($C$4:$C$7,$F$4:$F$7)</f>
-        <v>0.31578947368421051</v>
-      </c>
-      <c r="H4" s="19">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H4" s="16">
         <f>F4-D4</f>
-        <v>-10</v>
-      </c>
-      <c r="I4" s="5">
-        <v>1</v>
-      </c>
-      <c r="J4" s="30">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f>I4*C4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="22">
+        <f>(1-I4)*C4</f>
         <v>10</v>
       </c>
-      <c r="K4" s="27">
-        <f>(1-I4)*C4</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <f>K4*F4/SUMPRODUCT($K$4:$K$9,$F$4:$F$9)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="29">
+        <v>0.33333333042740032</v>
+      </c>
+      <c r="M4" s="24">
         <v>0.08</v>
       </c>
       <c r="N4" t="str">
         <f>IF($B$1-E4&gt;=365,"long term","short term")</f>
         <v>long term</v>
       </c>
-      <c r="O4" s="27">
+      <c r="O4" s="22">
         <f>I4*C4*H4</f>
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="R4" t="s">
         <v>30</v>
       </c>
       <c r="S4">
         <f>SUMIF(N4:N7,"=long term",O4:O7)</f>
-        <v>-100</v>
-      </c>
-      <c r="T4" s="27">
+        <v>0</v>
+      </c>
+      <c r="T4" s="22">
         <f>IF(S3*S4&lt;0,IF(S3&gt;-S4,0,S3+S4),S4)</f>
-        <v>-71.666666859862801</v>
-      </c>
-      <c r="V4">
-        <f>T4*0.35</f>
-        <v>-25.083333400951979</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>T4*0.15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>160</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="14">
         <f>$B$1-200</f>
         <v>45556</v>
       </c>
-      <c r="F5" s="17">
-        <v>180</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="12">
+        <v>200</v>
+      </c>
+      <c r="G5" s="11">
         <f t="shared" ref="G5:G7" si="0">C5*F5/SUMPRODUCT($C$4:$C$7,$F$4:$F$7)</f>
-        <v>0.15789473684210525</v>
-      </c>
-      <c r="H5" s="19">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="H5" s="16">
         <f t="shared" ref="H5:H7" si="1">F5-D5</f>
-        <v>20</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="30">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f t="shared" ref="J5:J7" si="2">I5*C5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="27">
+      <c r="K5" s="22">
         <f t="shared" ref="K5:K7" si="3">(1-I5)*C5</f>
         <v>5</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <f t="shared" ref="L5:L9" si="4">K5*F5/SUMPRODUCT($K$4:$K$9,$F$4:$F$9)</f>
-        <v>0.15789473671611209</v>
-      </c>
-      <c r="M5" s="29">
+        <v>0.16666666521370016</v>
+      </c>
+      <c r="M5" s="24">
         <v>0.08</v>
       </c>
       <c r="N5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="22">
         <f t="shared" ref="O5:O7" si="5">I5*C5*H5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>8</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>250</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="14">
         <f>$B$1-500</f>
         <v>45256</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="12">
         <v>300</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
-        <v>0.42105263157894735</v>
-      </c>
-      <c r="H6" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="16">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="30">
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="22">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <f t="shared" si="4"/>
-        <v>0.42105263124296555</v>
-      </c>
-      <c r="M6" s="29">
+        <v>0.39999999651288037</v>
+      </c>
+      <c r="M6" s="24">
         <v>0.12</v>
       </c>
       <c r="N6" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <v>2</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>280</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="19">
         <f>$B$1-100</f>
         <v>45656</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="17">
         <v>300</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="20">
         <f t="shared" si="0"/>
-        <v>0.10526315789473684</v>
-      </c>
-      <c r="H7" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="21">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I7" s="5">
-        <v>0.70833332850343012</v>
-      </c>
-      <c r="J7" s="30">
+      <c r="I7" s="4">
+        <v>0.48245612814030098</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="2"/>
-        <v>1.4166666570068602</v>
-      </c>
-      <c r="K7" s="27">
+        <v>0.96491225628060195</v>
+      </c>
+      <c r="K7" s="22">
         <f t="shared" si="3"/>
-        <v>0.58333334299313977</v>
-      </c>
-      <c r="L7" s="4">
+        <v>1.0350877437193979</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="4"/>
-        <v>3.0701754869877102E-2</v>
-      </c>
-      <c r="M7" s="29">
+        <v>5.1754386734785544E-2</v>
+      </c>
+      <c r="M7" s="24">
         <v>0.12</v>
       </c>
       <c r="N7" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="22">
         <f t="shared" si="5"/>
-        <v>28.333333140137206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>19.298245125612038</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="2">
-        <v>180</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="28">
-        <v>12.361111120280066</v>
-      </c>
-      <c r="L8" s="4">
+      <c r="F8" s="12">
+        <v>200</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="K8" s="23">
+        <v>1.4473685610220886</v>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="4"/>
-        <v>0.39035087717104522</v>
-      </c>
-      <c r="M8" s="29">
+        <v>4.8245618280140679E-2</v>
+      </c>
+      <c r="M8" s="24">
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="12">
         <v>300</v>
       </c>
-      <c r="K9" s="28">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
+      <c r="K9" s="23">
+        <v>5.6621855467300016E-8</v>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="29">
+        <v>2.8310927486841029E-9</v>
+      </c>
+      <c r="M9" s="24">
         <v>0.12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="F10" s="2"/>
-      <c r="K10" s="26"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="F11">
         <f>SUMPRODUCT($C$4:$C$9,$F$4:$F$9)</f>
-        <v>5700</v>
+        <v>6000</v>
       </c>
       <c r="K11">
         <f>SUMPRODUCT($F$4:$F$9,$K$4:$K$9)</f>
-        <v>5700.0000045483539</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+        <v>6000.0000523067947</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f>SUMPRODUCT(L4:L9,M4:M9)</f>
-        <v>9.8070175444513713E-2</v>
+        <v>9.8070175443150345E-2</v>
       </c>
       <c r="M13" t="s">
         <v>26</v>
@@ -1065,20 +1055,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4">
-        <f>(V3+V4)/F11</f>
-        <v>-4.4005848071845578E-3</v>
+      <c r="C14" s="3">
+        <f>(U3+U4)/F11</f>
+        <v>1.1257309656607021E-3</v>
       </c>
       <c r="L14" t="s">
         <v>1</v>
       </c>
       <c r="M14">
         <f>L4+L5+L8</f>
-        <v>0.54824561388715731</v>
+        <v>0.54824561392124116</v>
       </c>
       <c r="O14" t="s">
         <v>1</v>
@@ -1090,20 +1080,20 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>M14*M14*P14+M15*M15*Q15+2*P15*M14*M15</f>
-        <v>7.552997076491838E-2</v>
+        <v>7.5529970763839036E-2</v>
       </c>
       <c r="L15" t="s">
         <v>3</v>
       </c>
       <c r="M15">
         <f>L6+L7+L9</f>
-        <v>0.45175438611284263</v>
+        <v>0.45175438607875867</v>
       </c>
       <c r="O15" t="s">
         <v>3</v>
@@ -1119,9 +1109,9 @@
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="25">
         <f>C13-C14-2*C15</f>
-        <v>-4.8589181278138494E-2</v>
+        <v>-5.4115497050188421E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1131,41 +1121,41 @@
       <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <f>G4+G5</f>
-        <v>0.47368421052631576</v>
-      </c>
-      <c r="C20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="3">
         <f>L4+L5+L8</f>
-        <v>0.54824561388715731</v>
-      </c>
-      <c r="I20" s="4"/>
+        <v>0.54824561392124116</v>
+      </c>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <f>G6+G7</f>
-        <v>0.52631578947368418</v>
-      </c>
-      <c r="C21" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="3">
         <f>L6+L7+L9</f>
-        <v>0.45175438611284263</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>0.45175438607875867</v>
+      </c>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I22" s="4"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I23" s="4"/>
+      <c r="I23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>